<commit_message>
reg file fixed bugs and first CB implementation
</commit_message>
<xml_diff>
--- a/Work plan.xlsx
+++ b/Work plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liora.000\Documents\Semester Summer 19\Project\project_k_means\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edi12\OneDrive\שולחן העבודה\סמסטר 7\פרויקט א\k means project\project_k_means\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18F6531-15D6-404B-96DD-2BC740D2CDD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{D18F6531-15D6-404B-96DD-2BC740D2CDD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D576969A-AC1C-43EC-BF10-1775FDF48E70}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C2D5FB72-92D2-49F7-B1CB-0400004466DF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C2D5FB72-92D2-49F7-B1CB-0400004466DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Week</t>
   </si>
@@ -112,6 +112,12 @@
 User's instructions
 Verification section
 Doing final presentation</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -122,7 +128,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -170,7 +176,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -466,20 +472,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A51FB4-7F85-42C1-BC71-B74F499AC1A3}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,8 +495,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -500,8 +509,11 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -512,7 +524,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -523,7 +535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -534,7 +546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -545,7 +557,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -556,7 +568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -567,7 +579,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -578,7 +590,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -589,7 +601,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -600,7 +612,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -611,7 +623,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -622,7 +634,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -633,7 +645,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="56" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -644,7 +656,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>